<commit_message>
Revert "notes from conversation"
This reverts commit ba90a9467541accca0209198ca8a3eb358acdc9e.
</commit_message>
<xml_diff>
--- a/CFE 2018 Lending Analytics Competition Data Dictionary Final.xlsx
+++ b/CFE 2018 Lending Analytics Competition Data Dictionary Final.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20904"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jusitn\Documents\GitHub\CFE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\CFE 2018 Lending Analytics Competition\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4079667A-3F3D-4798-B10B-45C3DADD67E0}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="11_38C276D314AEEC598CD2F46C6ADF09614DF1946B" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8805" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8808" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="123">
   <si>
     <t>CFE 2018 Lending Analytics Competition</t>
   </si>
@@ -394,85 +394,13 @@
   </si>
   <si>
     <t>Promotion which runs for a limited time; intended to encourage refinances with CFE</t>
-  </si>
-  <si>
-    <t>Notes</t>
-  </si>
-  <si>
-    <t>Do not include in analysis</t>
-  </si>
-  <si>
-    <t>Target</t>
-  </si>
-  <si>
-    <t>Turn into Factor / Categorical</t>
-  </si>
-  <si>
-    <t>Requires format</t>
-  </si>
-  <si>
-    <t>Segregate data into co-applicant Yes / No
-Scale? 
-How to handle no credit history</t>
-  </si>
-  <si>
-    <t>Integer
-Scale?</t>
-  </si>
-  <si>
-    <t>Examine outliers; 
-consider cut-off = 0 &lt; min wage?</t>
-  </si>
-  <si>
-    <t>Add category for rent / liability &gt; income</t>
-  </si>
-  <si>
-    <t>Examine the "Zero / Null" cases</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Change "0" to N/A or Null
-Categorical or numerical?  Split into categories?
-Create new column for Compare loan applicant date.
-Year will equal current year if the specific vehicle is unknown. </t>
-  </si>
-  <si>
-    <t>Make this field required?</t>
-  </si>
-  <si>
-    <t>Logical gap between this field, milieage and Vehicle year.</t>
-  </si>
-  <si>
-    <t>Set = Amount Requested if unknown
-Requires formatting / assumptions.
-Impute from Blue-book values</t>
-  </si>
-  <si>
-    <t>Categorical</t>
-  </si>
-  <si>
-    <t>Ensure this data makes sense.
-May be able to impute based on loan size, down payment and duration.</t>
-  </si>
-  <si>
-    <t>Possilbe to conslidate field?</t>
-  </si>
-  <si>
-    <t>Loan to non-members?  Maybe not include in analysis.</t>
-  </si>
-  <si>
-    <t>Compare to reported values on liabilities?  Indicate additional evaluation from a person?
-Do histogram</t>
-  </si>
-  <si>
-    <t>This field should be calculated, NOT a required field.
-Investigate more - see histogram.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -503,14 +431,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -520,12 +442,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF002060"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -542,76 +458,70 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="11">
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF002060"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -635,7 +545,7 @@
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -659,7 +569,7 @@
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -683,7 +593,7 @@
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -707,7 +617,7 @@
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -731,7 +641,7 @@
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -781,42 +691,6 @@
       </fill>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF002060"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -831,26 +705,25 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="A5:F41" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
-  <autoFilter ref="A5:F41" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
-  <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Field" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Definition" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Calculation" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Required" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Remarks" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{A497DF00-E10A-42BB-8A4E-356430E02172}" name="Notes" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="A5:E41" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
+  <autoFilter ref="A5:E41" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Field" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Definition" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Calculation" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Required" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Remarks" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium20" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table1" displayName="Table1" ref="A47:B57" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table1" displayName="Table1" ref="A47:B57" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2">
   <autoFilter ref="A47:B57" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Request Type" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Description" dataDxfId="8"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Request Type" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Description" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium20" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1119,852 +992,750 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F57"/>
+  <dimension ref="A1:E57"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="1" ySplit="5" topLeftCell="C33" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="E37" sqref="E37"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="90" zoomScaleNormal="90" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
+      <selection activeCell="A59" sqref="A59"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="28.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="28.28515625" defaultRowHeight="14.45"/>
   <cols>
-    <col min="1" max="1" width="28.85546875" style="3" customWidth="1"/>
-    <col min="2" max="2" width="27.42578125" style="9" customWidth="1"/>
-    <col min="3" max="3" width="17.7109375" style="9" customWidth="1"/>
-    <col min="4" max="4" width="26.85546875" style="9" customWidth="1"/>
-    <col min="5" max="5" width="23.7109375" style="9" customWidth="1"/>
-    <col min="6" max="6" width="28.28515625" style="9"/>
+    <col min="2" max="2" width="76.7109375" customWidth="1"/>
+    <col min="3" max="3" width="68.7109375" customWidth="1"/>
+    <col min="4" max="4" width="70.5703125" customWidth="1"/>
+    <col min="5" max="5" width="110.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:5" ht="23.45">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-    </row>
-    <row r="2" spans="1:6" ht="13.9" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:6" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+    </row>
+    <row r="2" spans="1:5" ht="13.9" customHeight="1"/>
+    <row r="3" spans="1:5" ht="13.9" customHeight="1">
+      <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="13.9" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
+    <row r="4" spans="1:5" ht="13.9" customHeight="1"/>
+    <row r="5" spans="1:5" s="2" customFormat="1">
+      <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="E5" s="10" t="s">
+      <c r="D5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="10" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A6" s="5" t="s">
+    </row>
+    <row r="6" spans="1:5" s="3" customFormat="1" ht="13.9">
+      <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="F6" s="12" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A7" s="5" t="s">
+      <c r="C6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" s="3" customFormat="1" ht="13.9">
+      <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="F7" s="12" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" s="2" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A8" s="5" t="s">
+      <c r="C7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" s="3" customFormat="1" ht="13.9">
+      <c r="A8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="E8" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="F8" s="12" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" s="2" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A9" s="5" t="s">
+      <c r="D8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" s="3" customFormat="1" ht="13.9">
+      <c r="A9" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D9" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="E9" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="F9" s="12" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" s="2" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A10" s="5" t="s">
+      <c r="C9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" s="3" customFormat="1" ht="13.9">
+      <c r="A10" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="D10" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E10" s="8" t="s">
+      <c r="E10" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F10" s="12" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" s="2" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
-      <c r="A11" s="5" t="s">
+    </row>
+    <row r="11" spans="1:5" s="3" customFormat="1" ht="13.9">
+      <c r="A11" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="C11" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="D11" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E11" s="8" t="s">
+      <c r="E11" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F11" s="12" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" s="2" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A12" s="5" t="s">
+    </row>
+    <row r="12" spans="1:5" s="3" customFormat="1" ht="13.9">
+      <c r="A12" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C12" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D12" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="E12" s="8" t="s">
+      <c r="C12" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E12" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="F12" s="12" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" s="2" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A13" s="5" t="s">
+    </row>
+    <row r="13" spans="1:5" s="3" customFormat="1" ht="13.9">
+      <c r="A13" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C13" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D13" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="E13" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="F13" s="12" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" s="2" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A14" s="5" t="s">
+      <c r="C13" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" s="3" customFormat="1" ht="13.9">
+      <c r="A14" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C14" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D14" s="8" t="s">
+      <c r="C14" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E14" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="F14" s="12" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" s="2" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A15" s="5" t="s">
+      <c r="E14" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" s="3" customFormat="1" ht="13.9">
+      <c r="A15" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C15" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D15" s="8" t="s">
+      <c r="C15" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D15" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E15" s="8" t="s">
+      <c r="E15" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="F15" s="12" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" s="2" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A16" s="5" t="s">
+    </row>
+    <row r="16" spans="1:5" s="3" customFormat="1" ht="13.9">
+      <c r="A16" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C16" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D16" s="8" t="s">
+      <c r="C16" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D16" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E16" s="8" t="s">
+      <c r="E16" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="F16" s="12" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A17" s="5" t="s">
+    </row>
+    <row r="17" spans="1:5" s="3" customFormat="1" ht="13.9">
+      <c r="A17" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="B17" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C17" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D17" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="E17" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="F17" s="12" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A18" s="5" t="s">
+      <c r="C17" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" s="3" customFormat="1" ht="13.9">
+      <c r="A18" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="B18" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C18" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D18" s="8" t="s">
+      <c r="C18" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D18" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E18" s="8" t="s">
+      <c r="E18" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="F18" s="12" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" s="2" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A19" s="5" t="s">
+    </row>
+    <row r="19" spans="1:5" s="3" customFormat="1" ht="13.9">
+      <c r="A19" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B19" s="8" t="s">
+      <c r="B19" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C19" s="8" t="s">
+      <c r="C19" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D19" s="8" t="s">
+      <c r="D19" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E19" s="8" t="s">
+      <c r="E19" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F19" s="12" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A20" s="5" t="s">
+    </row>
+    <row r="20" spans="1:5" s="3" customFormat="1" ht="13.9">
+      <c r="A20" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B20" s="8" t="s">
+      <c r="B20" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C20" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D20" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="E20" s="8" t="s">
+      <c r="C20" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E20" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="F20" s="12" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" s="2" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A21" s="5" t="s">
+    </row>
+    <row r="21" spans="1:5" s="3" customFormat="1" ht="13.9">
+      <c r="A21" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B21" s="8" t="s">
+      <c r="B21" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C21" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D21" s="8" t="s">
+      <c r="C21" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D21" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E21" s="8" t="s">
+      <c r="E21" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="F21" s="12" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" s="2" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A22" s="5" t="s">
+    </row>
+    <row r="22" spans="1:5" s="3" customFormat="1" ht="13.9">
+      <c r="A22" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B22" s="8" t="s">
+      <c r="B22" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C22" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D22" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="E22" s="8" t="s">
+      <c r="C22" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E22" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="F22" s="12"/>
-    </row>
-    <row r="23" spans="1:6" s="2" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A23" s="5" t="s">
+    </row>
+    <row r="23" spans="1:5" s="3" customFormat="1" ht="13.9">
+      <c r="A23" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B23" s="8" t="s">
+      <c r="B23" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="C23" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D23" s="8" t="s">
+      <c r="C23" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D23" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E23" s="8" t="s">
+      <c r="E23" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="F23" s="12"/>
-    </row>
-    <row r="24" spans="1:6" s="2" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A24" s="5" t="s">
+    </row>
+    <row r="24" spans="1:5" s="3" customFormat="1" ht="13.9">
+      <c r="A24" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="B24" s="8" t="s">
+      <c r="B24" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C24" s="8" t="s">
+      <c r="C24" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D24" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="E24" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="F24" s="12" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" s="2" customFormat="1" ht="89.25" x14ac:dyDescent="0.2">
-      <c r="A25" s="5" t="s">
+      <c r="D24" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" s="3" customFormat="1" ht="13.9">
+      <c r="A25" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B25" s="8" t="s">
+      <c r="B25" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C25" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D25" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="E25" s="8" t="s">
+      <c r="C25" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E25" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="F25" s="12" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" s="2" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A26" s="5" t="s">
+    </row>
+    <row r="26" spans="1:5" s="3" customFormat="1" ht="13.9">
+      <c r="A26" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B26" s="8" t="s">
+      <c r="B26" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="C26" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D26" s="8" t="s">
+      <c r="C26" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D26" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E26" s="8" t="s">
+      <c r="E26" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="F26" s="12" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" s="2" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A27" s="5" t="s">
+    </row>
+    <row r="27" spans="1:5" s="3" customFormat="1" ht="13.9">
+      <c r="A27" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="B27" s="8" t="s">
+      <c r="B27" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="C27" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D27" s="8" t="s">
+      <c r="C27" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D27" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E27" s="8" t="s">
+      <c r="E27" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="F27" s="12" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" s="2" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A28" s="5" t="s">
+    </row>
+    <row r="28" spans="1:5" s="3" customFormat="1" ht="13.9">
+      <c r="A28" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="B28" s="8" t="s">
+      <c r="B28" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C28" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D28" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="E28" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="F28" s="12" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" s="2" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A29" s="5" t="s">
+      <c r="C28" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" s="3" customFormat="1" ht="13.9">
+      <c r="A29" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B29" s="8" t="s">
+      <c r="B29" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="C29" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D29" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="E29" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="F29" s="12" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A30" s="5" t="s">
+      <c r="C29" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" s="3" customFormat="1" ht="13.9">
+      <c r="A30" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="B30" s="8" t="s">
+      <c r="B30" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="C30" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D30" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="E30" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="F30" s="13"/>
-    </row>
-    <row r="31" spans="1:6" s="2" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A31" s="5" t="s">
+      <c r="C30" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" s="3" customFormat="1" ht="13.9">
+      <c r="A31" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="B31" s="8" t="s">
+      <c r="B31" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="C31" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D31" s="8" t="s">
+      <c r="C31" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D31" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E31" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="F31" s="13"/>
-    </row>
-    <row r="32" spans="1:6" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A32" s="5" t="s">
+      <c r="E31" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" s="3" customFormat="1" ht="13.9">
+      <c r="A32" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="B32" s="8" t="s">
+      <c r="B32" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="C32" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D32" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="E32" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="F32" s="13"/>
-    </row>
-    <row r="33" spans="1:6" s="2" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A33" s="5" t="s">
+      <c r="C32" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" s="3" customFormat="1" ht="13.9">
+      <c r="A33" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="B33" s="8" t="s">
+      <c r="B33" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="C33" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D33" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="E33" s="8" t="s">
+      <c r="C33" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E33" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="F33" s="12" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" s="2" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A34" s="5" t="s">
+    </row>
+    <row r="34" spans="1:5" s="3" customFormat="1" ht="13.9">
+      <c r="A34" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B34" s="8" t="s">
+      <c r="B34" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="C34" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D34" s="8" t="s">
+      <c r="C34" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D34" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E34" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="F34" s="13"/>
-    </row>
-    <row r="35" spans="1:6" s="2" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A35" s="5" t="s">
+      <c r="E34" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" s="3" customFormat="1" ht="13.9">
+      <c r="A35" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="B35" s="8" t="s">
+      <c r="B35" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="C35" s="8" t="s">
+      <c r="C35" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="D35" s="8" t="s">
+      <c r="D35" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="E35" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="F35" s="12" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" s="2" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
-      <c r="A36" s="5" t="s">
+      <c r="E35" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" s="3" customFormat="1" ht="13.9">
+      <c r="A36" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="B36" s="8" t="s">
+      <c r="B36" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="C36" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D36" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="E36" s="8" t="s">
+      <c r="C36" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E36" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="F36" s="13"/>
-    </row>
-    <row r="37" spans="1:6" s="2" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A37" s="5" t="s">
+    </row>
+    <row r="37" spans="1:5" s="3" customFormat="1" ht="13.9">
+      <c r="A37" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="B37" s="8" t="s">
+      <c r="B37" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="C37" s="8" t="s">
+      <c r="C37" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="D37" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="E37" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="F37" s="14" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" s="2" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A38" s="5" t="s">
+      <c r="D37" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" s="3" customFormat="1" ht="13.9">
+      <c r="A38" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="B38" s="8" t="s">
+      <c r="B38" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="C38" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D38" s="8" t="s">
+      <c r="C38" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D38" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E38" s="8" t="s">
+      <c r="E38" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="F38" s="12" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" s="2" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A39" s="5" t="s">
+    </row>
+    <row r="39" spans="1:5" s="3" customFormat="1" ht="13.9">
+      <c r="A39" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="B39" s="8" t="s">
+      <c r="B39" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="C39" s="8" t="s">
+      <c r="C39" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="D39" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="E39" s="8" t="s">
+      <c r="D39" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E39" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="F39" s="14" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A40" s="5" t="s">
+    </row>
+    <row r="40" spans="1:5" s="3" customFormat="1" ht="13.9">
+      <c r="A40" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="B40" s="8" t="s">
+      <c r="B40" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="C40" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D40" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="E40" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="F40" s="12" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" ht="39" x14ac:dyDescent="0.25">
-      <c r="A41" s="5" t="s">
+      <c r="C40" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="B41" s="8" t="s">
+      <c r="B41" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="C41" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D41" s="8" t="s">
+      <c r="C41" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D41" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E41" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="F41" s="12" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="7" t="s">
+      <c r="E41" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
+      <c r="A47" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="B47" s="11" t="s">
+      <c r="B47" s="5" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A48" s="3" t="s">
+    <row r="48" spans="1:5">
+      <c r="A48" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="B48" s="9" t="s">
+      <c r="B48" s="7" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="49" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A49" s="3" t="s">
+    <row r="49" spans="1:2">
+      <c r="A49" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="B49" s="9" t="s">
+      <c r="B49" s="7" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="50" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A50" s="3" t="s">
+    <row r="50" spans="1:2">
+      <c r="A50" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="B50" s="9" t="s">
+      <c r="B50" s="7" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="51" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A51" s="3" t="s">
+    <row r="51" spans="1:2">
+      <c r="A51" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="B51" s="9" t="s">
+      <c r="B51" s="7" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="52" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A52" s="3" t="s">
+    <row r="52" spans="1:2">
+      <c r="A52" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="B52" s="9" t="s">
+      <c r="B52" s="7" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="53" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A53" s="3" t="s">
+    <row r="53" spans="1:2">
+      <c r="A53" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="B53" s="9" t="s">
+      <c r="B53" s="7" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="54" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A54" s="3" t="s">
+    <row r="54" spans="1:2">
+      <c r="A54" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="B54" s="9" t="s">
+      <c r="B54" s="7" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="55" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A55" s="3" t="s">
+    <row r="55" spans="1:2">
+      <c r="A55" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="B55" s="9" t="s">
+      <c r="B55" s="7" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="56" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A56" s="3" t="s">
+    <row r="56" spans="1:2">
+      <c r="A56" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="B56" s="9" t="s">
+      <c r="B56" s="7" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="57" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A57" s="3" t="s">
+    <row r="57" spans="1:2">
+      <c r="A57" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="B57" s="9" t="s">
+      <c r="B57" s="7" t="s">
         <v>122</v>
       </c>
     </row>

</xml_diff>